<commit_message>
Default values for all settings are now written during the import
</commit_message>
<xml_diff>
--- a/db/bootstrap.xlsx
+++ b/db/bootstrap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LEHRER" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
   <si>
     <t>lehrer_id</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>wert</t>
+  </si>
+  <si>
+    <t>adminPassword</t>
+  </si>
+  <si>
+    <t>change_me</t>
   </si>
   <si>
     <t>endTime</t>
@@ -343,10 +349,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.74898785425101"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4574898785425"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.8421052631579"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.74898785425101"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.1336032388664"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.2267206477733"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.1336032388664"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -432,9 +438,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.74898785425101"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.7246963562753"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.74898785425101"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.1336032388664"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1336032388664"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -838,9 +844,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.74898785425101"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.2914979757085"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.74898785425101"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.1336032388664"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.59919028340081"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1336032388664"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1307,17 +1313,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2024291497976"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.4331983805668"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.74898785425101"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.7408906882591"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1336032388664"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1328,7 +1334,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>65</v>
       </c>
@@ -1352,6 +1358,15 @@
         <v>70</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1376,9 +1391,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2024291497976"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.66801619433198"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.74898785425101"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.7408906882591"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.0566801619433"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1336032388664"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1407,16 +1422,16 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2024291497976"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.66801619433198"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.582995951417"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.74898785425101"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.7408906882591"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.0566801619433"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.1336032388664"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Moved the teacher selection list to a dropdown menu
</commit_message>
<xml_diff>
--- a/db/bootstrap.xlsx
+++ b/db/bootstrap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LEHRER" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
   <si>
     <t>lehrer_id</t>
   </si>
@@ -36,18 +36,30 @@
     <t>raum</t>
   </si>
   <si>
+    <t>klassen</t>
+  </si>
+  <si>
     <t>Max Mustermann</t>
   </si>
   <si>
     <t>Klasse 1A</t>
   </si>
   <si>
+    <t>1A,2B</t>
+  </si>
+  <si>
     <t>schueler_id</t>
   </si>
   <si>
+    <t>klasse</t>
+  </si>
+  <si>
     <t>John Doe</t>
   </si>
   <si>
+    <t>1A</t>
+  </si>
+  <si>
     <t>zeit_id</t>
   </si>
   <si>
@@ -231,19 +243,19 @@
     <t>endTime</t>
   </si>
   <si>
-    <t>03.12.2014 (08:00 Uhr)</t>
+    <t>?? Nov. 2016 (07:30 Uhr)</t>
   </si>
   <si>
     <t>isLocked</t>
   </si>
   <si>
-    <t>false</t>
+    <t>true</t>
   </si>
   <si>
     <t>startTime</t>
   </si>
   <si>
-    <t>4. Dezember 2014 (14:00 - 19:00 Uhr)</t>
+    <t>?? Nov. 2016 (14:00 - 19:00 Uhr)</t>
   </si>
 </sst>
 </file>
@@ -341,18 +353,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.1336032388664"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.9919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.2267206477733"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.51417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.0647773279352"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.6842105263158"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.51417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -365,16 +377,22 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -430,25 +448,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.1336032388664"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0242914979757"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.51417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.4008097165992"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.51417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -456,7 +477,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -844,17 +868,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.1336032388664"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.59919028340081"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.51417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.90688259109312"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.51417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -862,7 +886,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -870,7 +894,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,7 +902,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -886,7 +910,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -894,7 +918,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -902,7 +926,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -910,7 +934,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -918,7 +942,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -926,7 +950,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -934,7 +958,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -942,7 +966,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -950,7 +974,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -958,7 +982,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -966,7 +990,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -974,7 +998,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -982,7 +1006,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -990,7 +1014,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -998,7 +1022,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1006,7 +1030,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1014,7 +1038,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1022,7 +1046,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1030,7 +1054,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1038,7 +1062,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,7 +1070,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1054,7 +1078,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1062,7 +1086,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1070,7 +1094,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1078,7 +1102,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1086,7 +1110,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1094,7 +1118,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1102,7 +1126,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1110,7 +1134,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1118,7 +1142,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1126,7 +1150,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1134,7 +1158,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1142,7 +1166,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1150,7 +1174,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1158,7 +1182,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1166,7 +1190,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1174,7 +1198,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1182,7 +1206,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1190,7 +1214,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1198,7 +1222,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1206,7 +1230,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1214,7 +1238,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1222,7 +1246,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1230,7 +1254,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1238,7 +1262,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1246,7 +1270,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1254,7 +1278,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1262,7 +1286,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1270,7 +1294,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1278,7 +1302,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,7 +1310,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1294,7 +1318,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1313,17 +1337,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.7408906882591"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.51417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1331,42 +1355,41 @@
         <v>1</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1391,9 +1414,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.7408906882591"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.0566801619433"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.5101214574899"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.51417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1401,7 +1424,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1428,10 +1451,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.7408906882591"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.0566801619433"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1983805668016"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.5101214574899"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.51417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1439,10 +1462,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Added login_code column to SCHUELER table
</commit_message>
<xml_diff>
--- a/db/bootstrap.xlsx
+++ b/db/bootstrap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LEHRER" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,237 +25,243 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
-  <si>
-    <t>lehrer_id</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>raum</t>
-  </si>
-  <si>
-    <t>klassen</t>
-  </si>
-  <si>
-    <t>Max Mustermann</t>
-  </si>
-  <si>
-    <t>Klasse 1A</t>
-  </si>
-  <si>
-    <t>1A,2B</t>
-  </si>
-  <si>
-    <t>schueler_id</t>
-  </si>
-  <si>
-    <t>klasse</t>
-  </si>
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>1A</t>
-  </si>
-  <si>
-    <t>zeit_id</t>
-  </si>
-  <si>
-    <t>zeit</t>
-  </si>
-  <si>
-    <t>14:00</t>
-  </si>
-  <si>
-    <t>14:05</t>
-  </si>
-  <si>
-    <t>14:10</t>
-  </si>
-  <si>
-    <t>14:15</t>
-  </si>
-  <si>
-    <t>14:20</t>
-  </si>
-  <si>
-    <t>14:25</t>
-  </si>
-  <si>
-    <t>14:30</t>
-  </si>
-  <si>
-    <t>14:35</t>
-  </si>
-  <si>
-    <t>14:40</t>
-  </si>
-  <si>
-    <t>14:45</t>
-  </si>
-  <si>
-    <t>14:50</t>
-  </si>
-  <si>
-    <t>15:00</t>
-  </si>
-  <si>
-    <t>15:05</t>
-  </si>
-  <si>
-    <t>15:10</t>
-  </si>
-  <si>
-    <t>15:15</t>
-  </si>
-  <si>
-    <t>15:20</t>
-  </si>
-  <si>
-    <t>15:25</t>
-  </si>
-  <si>
-    <t>15:30</t>
-  </si>
-  <si>
-    <t>15:35</t>
-  </si>
-  <si>
-    <t>15:40</t>
-  </si>
-  <si>
-    <t>15:45</t>
-  </si>
-  <si>
-    <t>15:50</t>
-  </si>
-  <si>
-    <t>16:00</t>
-  </si>
-  <si>
-    <t>16:05</t>
-  </si>
-  <si>
-    <t>16:10</t>
-  </si>
-  <si>
-    <t>16:15</t>
-  </si>
-  <si>
-    <t>16:20</t>
-  </si>
-  <si>
-    <t>16:25</t>
-  </si>
-  <si>
-    <t>16:30</t>
-  </si>
-  <si>
-    <t>16:35</t>
-  </si>
-  <si>
-    <t>16:40</t>
-  </si>
-  <si>
-    <t>16:45</t>
-  </si>
-  <si>
-    <t>16:50</t>
-  </si>
-  <si>
-    <t>17:00</t>
-  </si>
-  <si>
-    <t>17:05</t>
-  </si>
-  <si>
-    <t>17:10</t>
-  </si>
-  <si>
-    <t>17:15</t>
-  </si>
-  <si>
-    <t>17:20</t>
-  </si>
-  <si>
-    <t>17:25</t>
-  </si>
-  <si>
-    <t>17:30</t>
-  </si>
-  <si>
-    <t>17:35</t>
-  </si>
-  <si>
-    <t>17:40</t>
-  </si>
-  <si>
-    <t>17:45</t>
-  </si>
-  <si>
-    <t>17:50</t>
-  </si>
-  <si>
-    <t>18:00</t>
-  </si>
-  <si>
-    <t>18:05</t>
-  </si>
-  <si>
-    <t>18:10</t>
-  </si>
-  <si>
-    <t>18:15</t>
-  </si>
-  <si>
-    <t>18:20</t>
-  </si>
-  <si>
-    <t>18:25</t>
-  </si>
-  <si>
-    <t>18:30</t>
-  </si>
-  <si>
-    <t>18:35</t>
-  </si>
-  <si>
-    <t>18:40</t>
-  </si>
-  <si>
-    <t>18:45</t>
-  </si>
-  <si>
-    <t>18:50</t>
-  </si>
-  <si>
-    <t>wert</t>
-  </si>
-  <si>
-    <t>adminPassword</t>
-  </si>
-  <si>
-    <t>change_me</t>
-  </si>
-  <si>
-    <t>endTime</t>
-  </si>
-  <si>
-    <t>?? Nov. 2016 (07:30 Uhr)</t>
-  </si>
-  <si>
-    <t>isLocked</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>startTime</t>
-  </si>
-  <si>
-    <t>?? Nov. 2016 (14:00 - 19:00 Uhr)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="79">
+  <si>
+    <t xml:space="preserve">lehrer_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">klassen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max Mustermann</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klasse 1A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1A,2B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schueler_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">klasse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">login_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John Doe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zeit_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zeit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17:35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adminPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">change_me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?? Nov. 2016 (07:30 Uhr)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isLocked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">startTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?? Nov. 2016 (14:00 - 19:00 Uhr)</t>
   </si>
 </sst>
 </file>
@@ -263,7 +269,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -355,16 +361,16 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.51417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.0647773279352"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.6842105263158"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.51417004048583"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="9.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -435,7 +441,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -448,17 +454,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.51417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.4008097165992"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.51417004048583"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -471,16 +477,22 @@
       <c r="C1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -847,7 +859,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -862,23 +874,23 @@
   </sheetPr>
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.51417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.90688259109312"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.51417004048583"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -886,7 +898,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -894,7 +906,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -902,7 +914,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -910,7 +922,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -918,7 +930,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -926,7 +938,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -934,7 +946,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -942,7 +954,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -950,7 +962,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -958,7 +970,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -966,7 +978,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -974,7 +986,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -982,7 +994,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -990,7 +1002,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -998,7 +1010,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1006,7 +1018,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1014,7 +1026,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1022,7 +1034,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1030,7 +1042,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1038,7 +1050,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,7 +1058,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1054,7 +1066,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1062,7 +1074,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1070,7 +1082,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1078,7 +1090,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1086,7 +1098,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1094,7 +1106,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1102,7 +1114,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1110,7 +1122,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1118,7 +1130,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1126,7 +1138,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1134,7 +1146,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1142,7 +1154,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1150,7 +1162,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1158,7 +1170,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1166,7 +1178,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1174,7 +1186,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1182,7 +1194,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1190,7 +1202,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1198,7 +1210,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1206,7 +1218,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1214,7 +1226,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1222,7 +1234,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1230,7 +1242,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1238,7 +1250,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1246,7 +1258,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1254,7 +1266,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1262,7 +1274,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1270,7 +1282,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1278,7 +1290,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,7 +1298,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1294,7 +1306,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1302,7 +1314,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1310,7 +1322,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1318,13 +1330,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1339,15 +1351,15 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2753036437247"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.51417004048583"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1355,45 +1367,45 @@
         <v>1</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1408,15 +1420,15 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2753036437247"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.5101214574899"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.51417004048583"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1424,13 +1436,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1445,16 +1457,16 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2753036437247"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.5101214574899"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8906882591093"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.51417004048583"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="9.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1462,7 +1474,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>7</v>
@@ -1473,7 +1485,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>